<commit_message>
Atualizado os filtros no pandas
</commit_message>
<xml_diff>
--- a/disponibilidade/DISPONIBILIDADE_CONTRATO.xlsx
+++ b/disponibilidade/DISPONIBILIDADE_CONTRATO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="37710" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="amostras" sheetId="1" state="visible" r:id="rId1"/>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:T1431"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A687" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D687" sqref="D687"/>
+      <selection activeCell="A693" sqref="A693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -34334,26 +34334,56 @@
       <c r="A688" s="9" t="n">
         <v>45644</v>
       </c>
-      <c r="B688" s="17" t="n"/>
-      <c r="C688" s="17" t="n"/>
-      <c r="D688" s="16" t="n"/>
-      <c r="E688" s="17" t="n"/>
-      <c r="F688" s="17" t="n"/>
-      <c r="G688" s="16" t="n"/>
-      <c r="H688" s="17" t="n"/>
-      <c r="I688" s="17" t="n"/>
-      <c r="J688" s="16" t="n"/>
-      <c r="K688" s="17" t="n"/>
-      <c r="L688" s="17" t="n"/>
-      <c r="M688" s="16" t="n"/>
-      <c r="N688" s="17" t="n"/>
-      <c r="O688" s="17" t="n"/>
-      <c r="P688" s="16" t="n"/>
+      <c r="B688" s="17" t="n">
+        <v>1253</v>
+      </c>
+      <c r="C688" s="17" t="n">
+        <v>1365</v>
+      </c>
+      <c r="D688" s="16" t="n">
+        <v>91.79000000000001</v>
+      </c>
+      <c r="E688" s="17" t="n">
+        <v>1267</v>
+      </c>
+      <c r="F688" s="17" t="n">
+        <v>1365</v>
+      </c>
+      <c r="G688" s="16" t="n">
+        <v>92.82000000000001</v>
+      </c>
+      <c r="H688" s="17" t="n">
+        <v>1246</v>
+      </c>
+      <c r="I688" s="17" t="n">
+        <v>1365</v>
+      </c>
+      <c r="J688" s="16" t="n">
+        <v>91.28</v>
+      </c>
+      <c r="K688" s="17" t="n">
+        <v>1248</v>
+      </c>
+      <c r="L688" s="17" t="n">
+        <v>1365</v>
+      </c>
+      <c r="M688" s="16" t="n">
+        <v>91.43000000000001</v>
+      </c>
+      <c r="N688" s="17" t="n">
+        <v>1258</v>
+      </c>
+      <c r="O688" s="17" t="n">
+        <v>1365</v>
+      </c>
+      <c r="P688" s="16" t="n">
+        <v>92.16</v>
+      </c>
       <c r="Q688" s="17" t="n"/>
       <c r="R688" s="17" t="n"/>
       <c r="S688" s="16" t="n"/>
-      <c r="T688" s="11" t="e">
-        <v>#DIV/0!</v>
+      <c r="T688" s="11" t="n">
+        <v>91.896</v>
       </c>
     </row>
     <row r="689" ht="18.75" customHeight="1">
@@ -34464,12 +34494,24 @@
       <c r="A693" s="9" t="n">
         <v>45649</v>
       </c>
-      <c r="B693" s="17" t="n"/>
-      <c r="C693" s="17" t="n"/>
-      <c r="D693" s="16" t="n"/>
-      <c r="E693" s="17" t="n"/>
-      <c r="F693" s="17" t="n"/>
-      <c r="G693" s="16" t="n"/>
+      <c r="B693" s="17" t="n">
+        <v>1263</v>
+      </c>
+      <c r="C693" s="17" t="n">
+        <v>1360</v>
+      </c>
+      <c r="D693" s="16" t="n">
+        <v>92.86764705882354</v>
+      </c>
+      <c r="E693" s="17" t="n">
+        <v>1260</v>
+      </c>
+      <c r="F693" s="17" t="n">
+        <v>1360</v>
+      </c>
+      <c r="G693" s="16" t="n">
+        <v>92.64705882352942</v>
+      </c>
       <c r="H693" s="17" t="n"/>
       <c r="I693" s="17" t="n"/>
       <c r="J693" s="16" t="n"/>
@@ -34482,8 +34524,8 @@
       <c r="Q693" s="17" t="n"/>
       <c r="R693" s="17" t="n"/>
       <c r="S693" s="16" t="n"/>
-      <c r="T693" s="11" t="e">
-        <v>#DIV/0!</v>
+      <c r="T693" s="11" t="n">
+        <v>92.7574</v>
       </c>
     </row>
     <row r="694" ht="18.75" customHeight="1">
@@ -34516,9 +34558,15 @@
       <c r="A695" s="9" t="n">
         <v>45651</v>
       </c>
-      <c r="B695" s="17" t="n"/>
-      <c r="C695" s="17" t="n"/>
-      <c r="D695" s="16" t="n"/>
+      <c r="B695" s="17" t="n">
+        <v>1247</v>
+      </c>
+      <c r="C695" s="17" t="n">
+        <v>1360</v>
+      </c>
+      <c r="D695" s="16" t="n">
+        <v>91.69117647058823</v>
+      </c>
       <c r="E695" s="17" t="n"/>
       <c r="F695" s="17" t="n"/>
       <c r="G695" s="16" t="n"/>
@@ -34534,8 +34582,8 @@
       <c r="Q695" s="17" t="n"/>
       <c r="R695" s="17" t="n"/>
       <c r="S695" s="16" t="n"/>
-      <c r="T695" s="11" t="e">
-        <v>#DIV/0!</v>
+      <c r="T695" s="11" t="n">
+        <v>91.69117647058823</v>
       </c>
     </row>
     <row r="696" ht="18.75" customHeight="1">

</xml_diff>